<commit_message>
first try ANN model
</commit_message>
<xml_diff>
--- a/Step_1_Process_Yearbook_Data/02_Digitized_data/河南_2002.xlsx
+++ b/Step_1_Process_Yearbook_Data/02_Digitized_data/河南_2002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangj\Desktop\Agricultural_production\01_Yearbook_Data\02_Digitized_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangj\Desktop\Agricultural_production\Step_1_Process_Yearbook_Data\02_Digitized_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E518EF-AD2E-4E94-86C5-1C4F93E185B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA8E3C7-F6D3-4A72-9915-8E29AF4DA411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="2235" windowWidth="15855" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7635" yWindow="3780" windowWidth="15855" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2091,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3643,7 +3643,7 @@
         <v>116677</v>
       </c>
       <c r="D68" s="1">
-        <v>67.209999999999994</v>
+        <v>6727</v>
       </c>
       <c r="E68" s="1">
         <v>13.77</v>
@@ -3965,7 +3965,7 @@
         <v>221895</v>
       </c>
       <c r="D82" s="1">
-        <v>0.63270000000000004</v>
+        <v>6327</v>
       </c>
       <c r="E82" s="1">
         <v>25.37</v>
@@ -3988,7 +3988,7 @@
         <v>8695</v>
       </c>
       <c r="D83" s="7">
-        <v>0.55740000000000001</v>
+        <v>5574</v>
       </c>
       <c r="E83" s="1">
         <v>1.47</v>

</xml_diff>